<commit_message>
finalizando a estruturaçao das campanhas de Bing
</commit_message>
<xml_diff>
--- a/sheets/dados.xlsx
+++ b/sheets/dados.xlsx
@@ -18,7 +18,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -26,13 +26,23 @@
       <sz val="11"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <name val="Space Grotesk"/>
+      <b val="1"/>
+      <color rgb="00FFFFFF"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="004f24ee"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -47,8 +57,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -432,7 +445,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -441,55 +454,76 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" t="inlineStr">
+      <c r="A1" s="1" t="inlineStr">
         <is>
           <t>Bing Ads</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>Bing Ads</t>
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>[RCK] Search - Serviços</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>[RCK] Search - Serviços</t>
+          <t>Mes</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Investimento</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Impressoes</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Cliques</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>CPC</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>CTR</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Mes</t>
+          <t>Setembro</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Investimento</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>Impressoes</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>Cliques</t>
-        </is>
+          <t>R$ 484,12</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>28435</v>
+      </c>
+      <c r="D4" t="n">
+        <v>361</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>CPC</t>
+          <t>R$ 1,34</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>CTR</t>
+          <t>1.27%</t>
         </is>
       </c>
     </row>
@@ -501,100 +535,197 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>R$ 484,12</t>
+          <t>R$ 512,24</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>28435</v>
+        <v>25389</v>
       </c>
       <c r="D5" t="n">
-        <v>361</v>
+        <v>320</v>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>R$ 1,34</t>
+          <t>R$ 1,28</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>1.27%</t>
+          <t>1.32%</t>
         </is>
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="inlineStr"/>
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Variaçao</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>-0.05%</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>0.12%</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>0.13%</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>0.05%</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>-0.04%</t>
+        </is>
+      </c>
     </row>
     <row r="7">
-      <c r="A7" t="inlineStr">
+      <c r="A7" t="inlineStr"/>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="inlineStr">
         <is>
           <t>[RCK] Search - Institucional Jitterbit</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>Mes</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>Investimento</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>Impressoes</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>Cliques</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>CPC</t>
-        </is>
-      </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>CTR</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
+          <t>Mes</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Investimento</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Impressoes</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>Cliques</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>CPC</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>CTR</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
           <t>Setembro</t>
         </is>
       </c>
-      <c r="B9" t="inlineStr">
+      <c r="B10" t="inlineStr">
         <is>
           <t>R$ 3,12</t>
         </is>
       </c>
-      <c r="C9" t="n">
+      <c r="C10" t="n">
         <v>79</v>
       </c>
-      <c r="D9" t="n">
+      <c r="D10" t="n">
         <v>28</v>
       </c>
-      <c r="E9" t="inlineStr">
+      <c r="E10" t="inlineStr">
         <is>
           <t>R$ 0,11</t>
         </is>
       </c>
-      <c r="F9" t="inlineStr">
+      <c r="F10" t="inlineStr">
         <is>
           <t>35.44%</t>
         </is>
       </c>
     </row>
-    <row r="10">
-      <c r="A10" t="inlineStr"/>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Setembro</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>R$ 3,12</t>
+        </is>
+      </c>
+      <c r="C11" t="n">
+        <v>79</v>
+      </c>
+      <c r="D11" t="n">
+        <v>28</v>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>R$ 0,11</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>35.44%</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Variaçao</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>0.00%</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>0.00%</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>0.00%</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>0.00%</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>0.00%</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr"/>
     </row>
   </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A8:F8"/>
+    <mergeCell ref="A2:F2"/>
+    <mergeCell ref="A1:F1"/>
+  </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
[bugFix] ajustando a campanha anterior para pegar os dados do mes anterior
</commit_message>
<xml_diff>
--- a/sheets/dados.xlsx
+++ b/sheets/dados.xlsx
@@ -530,7 +530,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Setembro</t>
+          <t>Agosto</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -660,7 +660,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Setembro</t>
+          <t>Agosto</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">

</xml_diff>

<commit_message>
reestruturando as funçoes de criaçao de linhas
</commit_message>
<xml_diff>
--- a/sheets/dados.xlsx
+++ b/sheets/dados.xlsx
@@ -18,7 +18,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="2">
+  <fonts count="4">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -31,18 +31,19 @@
       <b val="1"/>
       <color rgb="00FFFFFF"/>
     </font>
+    <font>
+      <name val="Space Grotesk"/>
+    </font>
+    <font>
+      <b val="1"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="004f24ee"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -57,9 +58,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -468,127 +475,127 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
+      <c r="A3" s="2" t="inlineStr">
         <is>
           <t>Mes</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr">
+      <c r="B3" s="2" t="inlineStr">
         <is>
           <t>Investimento</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr">
+      <c r="C3" s="2" t="inlineStr">
         <is>
           <t>Impressoes</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr">
+      <c r="D3" s="2" t="inlineStr">
         <is>
           <t>Cliques</t>
         </is>
       </c>
-      <c r="E3" t="inlineStr">
+      <c r="E3" s="2" t="inlineStr">
         <is>
           <t>CPC</t>
         </is>
       </c>
-      <c r="F3" t="inlineStr">
+      <c r="F3" s="2" t="inlineStr">
         <is>
           <t>CTR</t>
         </is>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="inlineStr">
+      <c r="A4" s="2" t="inlineStr">
         <is>
           <t>Setembro</t>
         </is>
       </c>
-      <c r="B4" t="inlineStr">
+      <c r="B4" s="2" t="inlineStr">
         <is>
           <t>R$ 484,12</t>
         </is>
       </c>
-      <c r="C4" t="n">
+      <c r="C4" s="2" t="n">
         <v>28435</v>
       </c>
-      <c r="D4" t="n">
+      <c r="D4" s="2" t="n">
         <v>361</v>
       </c>
-      <c r="E4" t="inlineStr">
+      <c r="E4" s="2" t="inlineStr">
         <is>
           <t>R$ 1,34</t>
         </is>
       </c>
-      <c r="F4" t="inlineStr">
+      <c r="F4" s="2" t="inlineStr">
         <is>
           <t>1.27%</t>
         </is>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="inlineStr">
+      <c r="A5" s="2" t="inlineStr">
         <is>
           <t>Agosto</t>
         </is>
       </c>
-      <c r="B5" t="inlineStr">
+      <c r="B5" s="2" t="inlineStr">
         <is>
           <t>R$ 512,24</t>
         </is>
       </c>
-      <c r="C5" t="n">
+      <c r="C5" s="2" t="n">
         <v>25389</v>
       </c>
-      <c r="D5" t="n">
+      <c r="D5" s="2" t="n">
         <v>320</v>
       </c>
-      <c r="E5" t="inlineStr">
+      <c r="E5" s="2" t="inlineStr">
         <is>
           <t>R$ 1,28</t>
         </is>
       </c>
-      <c r="F5" t="inlineStr">
+      <c r="F5" s="2" t="inlineStr">
         <is>
           <t>1.32%</t>
         </is>
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="inlineStr">
+      <c r="A6" s="3" t="inlineStr">
         <is>
           <t>Variaçao</t>
         </is>
       </c>
-      <c r="B6" t="inlineStr">
+      <c r="B6" s="3" t="inlineStr">
         <is>
           <t>-0.05%</t>
         </is>
       </c>
-      <c r="C6" t="inlineStr">
+      <c r="C6" s="3" t="inlineStr">
         <is>
           <t>0.12%</t>
         </is>
       </c>
-      <c r="D6" t="inlineStr">
+      <c r="D6" s="3" t="inlineStr">
         <is>
           <t>0.13%</t>
         </is>
       </c>
-      <c r="E6" t="inlineStr">
+      <c r="E6" s="3" t="inlineStr">
         <is>
           <t>0.05%</t>
         </is>
       </c>
-      <c r="F6" t="inlineStr">
+      <c r="F6" s="3" t="inlineStr">
         <is>
           <t>-0.04%</t>
         </is>
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="inlineStr"/>
+      <c r="A7" s="2" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
@@ -598,127 +605,127 @@
       </c>
     </row>
     <row r="9">
-      <c r="A9" t="inlineStr">
+      <c r="A9" s="2" t="inlineStr">
         <is>
           <t>Mes</t>
         </is>
       </c>
-      <c r="B9" t="inlineStr">
+      <c r="B9" s="2" t="inlineStr">
         <is>
           <t>Investimento</t>
         </is>
       </c>
-      <c r="C9" t="inlineStr">
+      <c r="C9" s="2" t="inlineStr">
         <is>
           <t>Impressoes</t>
         </is>
       </c>
-      <c r="D9" t="inlineStr">
+      <c r="D9" s="2" t="inlineStr">
         <is>
           <t>Cliques</t>
         </is>
       </c>
-      <c r="E9" t="inlineStr">
+      <c r="E9" s="2" t="inlineStr">
         <is>
           <t>CPC</t>
         </is>
       </c>
-      <c r="F9" t="inlineStr">
+      <c r="F9" s="2" t="inlineStr">
         <is>
           <t>CTR</t>
         </is>
       </c>
     </row>
     <row r="10">
-      <c r="A10" t="inlineStr">
+      <c r="A10" s="2" t="inlineStr">
         <is>
           <t>Setembro</t>
         </is>
       </c>
-      <c r="B10" t="inlineStr">
+      <c r="B10" s="2" t="inlineStr">
         <is>
           <t>R$ 3,12</t>
         </is>
       </c>
-      <c r="C10" t="n">
+      <c r="C10" s="2" t="n">
         <v>79</v>
       </c>
-      <c r="D10" t="n">
+      <c r="D10" s="2" t="n">
         <v>28</v>
       </c>
-      <c r="E10" t="inlineStr">
+      <c r="E10" s="2" t="inlineStr">
         <is>
           <t>R$ 0,11</t>
         </is>
       </c>
-      <c r="F10" t="inlineStr">
+      <c r="F10" s="2" t="inlineStr">
         <is>
           <t>35.44%</t>
         </is>
       </c>
     </row>
     <row r="11">
-      <c r="A11" t="inlineStr">
+      <c r="A11" s="2" t="inlineStr">
         <is>
           <t>Agosto</t>
         </is>
       </c>
-      <c r="B11" t="inlineStr">
+      <c r="B11" s="2" t="inlineStr">
         <is>
           <t>R$ 3,12</t>
         </is>
       </c>
-      <c r="C11" t="n">
+      <c r="C11" s="2" t="n">
         <v>79</v>
       </c>
-      <c r="D11" t="n">
+      <c r="D11" s="2" t="n">
         <v>28</v>
       </c>
-      <c r="E11" t="inlineStr">
+      <c r="E11" s="2" t="inlineStr">
         <is>
           <t>R$ 0,11</t>
         </is>
       </c>
-      <c r="F11" t="inlineStr">
+      <c r="F11" s="2" t="inlineStr">
         <is>
           <t>35.44%</t>
         </is>
       </c>
     </row>
     <row r="12">
-      <c r="A12" t="inlineStr">
+      <c r="A12" s="3" t="inlineStr">
         <is>
           <t>Variaçao</t>
         </is>
       </c>
-      <c r="B12" t="inlineStr">
+      <c r="B12" s="3" t="inlineStr">
         <is>
           <t>0.00%</t>
         </is>
       </c>
-      <c r="C12" t="inlineStr">
+      <c r="C12" s="3" t="inlineStr">
         <is>
           <t>0.00%</t>
         </is>
       </c>
-      <c r="D12" t="inlineStr">
+      <c r="D12" s="3" t="inlineStr">
         <is>
           <t>0.00%</t>
         </is>
       </c>
-      <c r="E12" t="inlineStr">
+      <c r="E12" s="3" t="inlineStr">
         <is>
           <t>0.00%</t>
         </is>
       </c>
-      <c r="F12" t="inlineStr">
+      <c r="F12" s="3" t="inlineStr">
         <is>
           <t>0.00%</t>
         </is>
       </c>
     </row>
     <row r="13">
-      <c r="A13" t="inlineStr"/>
+      <c r="A13" s="2" t="inlineStr"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>

<commit_message>
excluindo automaticamente a planilha 'Sheets' que e criada pelo programa ao iniciar uma planilha
</commit_message>
<xml_diff>
--- a/sheets/dados.xlsx
+++ b/sheets/dados.xlsx
@@ -4,11 +4,10 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="1" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="Bing" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Bing" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -439,24 +438,6 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>

<commit_message>
recuperando as campanhas de linkedin e inserindo na planilha
</commit_message>
<xml_diff>
--- a/sheets/dados.xlsx
+++ b/sheets/dados.xlsx
@@ -4,10 +4,11 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="1" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Bing" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="LinkedIn" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -729,4 +730,956 @@
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:G50"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="15" customWidth="1" min="1" max="1"/>
+    <col width="15" customWidth="1" min="2" max="2"/>
+    <col width="15" customWidth="1" min="3" max="3"/>
+    <col width="15" customWidth="1" min="4" max="4"/>
+    <col width="15" customWidth="1" min="5" max="5"/>
+    <col width="15" customWidth="1" min="6" max="6"/>
+    <col width="15" customWidth="1" min="7" max="7"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="20" customHeight="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>LinkedIn Ads</t>
+        </is>
+      </c>
+    </row>
+    <row r="2" ht="25" customHeight="1">
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>[RCK] Campanha de Mensagem</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="2" t="inlineStr">
+        <is>
+          <t>Mes</t>
+        </is>
+      </c>
+      <c r="B3" s="2" t="inlineStr">
+        <is>
+          <t>Investimento</t>
+        </is>
+      </c>
+      <c r="C3" s="2" t="inlineStr">
+        <is>
+          <t>Impressoes</t>
+        </is>
+      </c>
+      <c r="D3" s="2" t="inlineStr">
+        <is>
+          <t>Cliques</t>
+        </is>
+      </c>
+      <c r="E3" s="2" t="inlineStr">
+        <is>
+          <t>CTR</t>
+        </is>
+      </c>
+      <c r="F3" s="2" t="inlineStr">
+        <is>
+          <t>CPC medio</t>
+        </is>
+      </c>
+      <c r="G3" s="2" t="inlineStr">
+        <is>
+          <t>Leads</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="3" t="inlineStr">
+        <is>
+          <t>Setembro</t>
+        </is>
+      </c>
+      <c r="B4" s="3" t="inlineStr">
+        <is>
+          <t>R$ 454,06</t>
+        </is>
+      </c>
+      <c r="C4" s="3" t="n">
+        <v>3309</v>
+      </c>
+      <c r="D4" s="3" t="n">
+        <v>3169</v>
+      </c>
+      <c r="E4" s="3" t="inlineStr">
+        <is>
+          <t>R$ 0,14328179236352162</t>
+        </is>
+      </c>
+      <c r="F4" s="3" t="n">
+        <v>0.9576911453611363</v>
+      </c>
+      <c r="G4" s="3" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="3" t="inlineStr">
+        <is>
+          <t>Agosto</t>
+        </is>
+      </c>
+      <c r="B5" s="3" t="inlineStr">
+        <is>
+          <t>R$ 454,06</t>
+        </is>
+      </c>
+      <c r="C5" s="3" t="n">
+        <v>3309</v>
+      </c>
+      <c r="D5" s="3" t="n">
+        <v>3169</v>
+      </c>
+      <c r="E5" s="3" t="inlineStr">
+        <is>
+          <t>R$ 0,14328179236352162</t>
+        </is>
+      </c>
+      <c r="F5" s="3" t="n">
+        <v>0.9576911453611363</v>
+      </c>
+      <c r="G5" s="3" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="3" t="inlineStr"/>
+    </row>
+    <row r="7">
+      <c r="A7" s="3" t="inlineStr">
+        <is>
+          <t>Agosto</t>
+        </is>
+      </c>
+      <c r="B7" s="3" t="inlineStr">
+        <is>
+          <t>R$ 453,91</t>
+        </is>
+      </c>
+      <c r="C7" s="3" t="n">
+        <v>2119</v>
+      </c>
+      <c r="D7" s="3" t="n">
+        <v>1962</v>
+      </c>
+      <c r="E7" s="3" t="inlineStr">
+        <is>
+          <t>R$ 0,2313506625891947</t>
+        </is>
+      </c>
+      <c r="F7" s="3" t="n">
+        <v>0.92590844738084</v>
+      </c>
+      <c r="G7" s="3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="3" t="inlineStr"/>
+    </row>
+    <row r="9">
+      <c r="A9" s="3" t="inlineStr">
+        <is>
+          <t>Agosto</t>
+        </is>
+      </c>
+      <c r="B9" s="3" t="inlineStr">
+        <is>
+          <t>R$ 452,48</t>
+        </is>
+      </c>
+      <c r="C9" s="3" t="n">
+        <v>995</v>
+      </c>
+      <c r="D9" s="3" t="n">
+        <v>1003</v>
+      </c>
+      <c r="E9" s="3" t="inlineStr">
+        <is>
+          <t>R$ 0,45112662013958127</t>
+        </is>
+      </c>
+      <c r="F9" s="3" t="n">
+        <v>1.008040201005025</v>
+      </c>
+      <c r="G9" s="3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="3" t="inlineStr"/>
+    </row>
+    <row r="11">
+      <c r="A11" s="3" t="inlineStr">
+        <is>
+          <t>Agosto</t>
+        </is>
+      </c>
+      <c r="B11" s="3" t="inlineStr">
+        <is>
+          <t>R$ 356,70</t>
+        </is>
+      </c>
+      <c r="C11" s="3" t="n">
+        <v>1986</v>
+      </c>
+      <c r="D11" s="3" t="n">
+        <v>2070</v>
+      </c>
+      <c r="E11" s="3" t="inlineStr">
+        <is>
+          <t>R$ 0,17231884057971014</t>
+        </is>
+      </c>
+      <c r="F11" s="3" t="n">
+        <v>1.042296072507553</v>
+      </c>
+      <c r="G11" s="3" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="3" t="inlineStr"/>
+    </row>
+    <row r="13" ht="25" customHeight="1">
+      <c r="A13" s="1" t="inlineStr">
+        <is>
+          <t>[RCK] Campanha de Mensagem</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="2" t="inlineStr">
+        <is>
+          <t>Mes</t>
+        </is>
+      </c>
+      <c r="B14" s="2" t="inlineStr">
+        <is>
+          <t>Investimento</t>
+        </is>
+      </c>
+      <c r="C14" s="2" t="inlineStr">
+        <is>
+          <t>Impressoes</t>
+        </is>
+      </c>
+      <c r="D14" s="2" t="inlineStr">
+        <is>
+          <t>Cliques</t>
+        </is>
+      </c>
+      <c r="E14" s="2" t="inlineStr">
+        <is>
+          <t>CTR</t>
+        </is>
+      </c>
+      <c r="F14" s="2" t="inlineStr">
+        <is>
+          <t>CPC medio</t>
+        </is>
+      </c>
+      <c r="G14" s="2" t="inlineStr">
+        <is>
+          <t>Leads</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="3" t="inlineStr">
+        <is>
+          <t>Setembro</t>
+        </is>
+      </c>
+      <c r="B15" s="3" t="inlineStr">
+        <is>
+          <t>R$ 453,91</t>
+        </is>
+      </c>
+      <c r="C15" s="3" t="n">
+        <v>2119</v>
+      </c>
+      <c r="D15" s="3" t="n">
+        <v>1962</v>
+      </c>
+      <c r="E15" s="3" t="inlineStr">
+        <is>
+          <t>R$ 0,2313506625891947</t>
+        </is>
+      </c>
+      <c r="F15" s="3" t="n">
+        <v>0.92590844738084</v>
+      </c>
+      <c r="G15" s="3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="3" t="inlineStr">
+        <is>
+          <t>Agosto</t>
+        </is>
+      </c>
+      <c r="B16" s="3" t="inlineStr">
+        <is>
+          <t>R$ 454,06</t>
+        </is>
+      </c>
+      <c r="C16" s="3" t="n">
+        <v>3309</v>
+      </c>
+      <c r="D16" s="3" t="n">
+        <v>3169</v>
+      </c>
+      <c r="E16" s="3" t="inlineStr">
+        <is>
+          <t>R$ 0,14328179236352162</t>
+        </is>
+      </c>
+      <c r="F16" s="3" t="n">
+        <v>0.9576911453611363</v>
+      </c>
+      <c r="G16" s="3" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="3" t="inlineStr"/>
+    </row>
+    <row r="18">
+      <c r="A18" s="3" t="inlineStr">
+        <is>
+          <t>Agosto</t>
+        </is>
+      </c>
+      <c r="B18" s="3" t="inlineStr">
+        <is>
+          <t>R$ 453,91</t>
+        </is>
+      </c>
+      <c r="C18" s="3" t="n">
+        <v>2119</v>
+      </c>
+      <c r="D18" s="3" t="n">
+        <v>1962</v>
+      </c>
+      <c r="E18" s="3" t="inlineStr">
+        <is>
+          <t>R$ 0,2313506625891947</t>
+        </is>
+      </c>
+      <c r="F18" s="3" t="n">
+        <v>0.92590844738084</v>
+      </c>
+      <c r="G18" s="3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="3" t="inlineStr"/>
+    </row>
+    <row r="20">
+      <c r="A20" s="3" t="inlineStr">
+        <is>
+          <t>Agosto</t>
+        </is>
+      </c>
+      <c r="B20" s="3" t="inlineStr">
+        <is>
+          <t>R$ 452,48</t>
+        </is>
+      </c>
+      <c r="C20" s="3" t="n">
+        <v>995</v>
+      </c>
+      <c r="D20" s="3" t="n">
+        <v>1003</v>
+      </c>
+      <c r="E20" s="3" t="inlineStr">
+        <is>
+          <t>R$ 0,45112662013958127</t>
+        </is>
+      </c>
+      <c r="F20" s="3" t="n">
+        <v>1.008040201005025</v>
+      </c>
+      <c r="G20" s="3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="3" t="inlineStr"/>
+    </row>
+    <row r="22">
+      <c r="A22" s="3" t="inlineStr">
+        <is>
+          <t>Agosto</t>
+        </is>
+      </c>
+      <c r="B22" s="3" t="inlineStr">
+        <is>
+          <t>R$ 356,70</t>
+        </is>
+      </c>
+      <c r="C22" s="3" t="n">
+        <v>1986</v>
+      </c>
+      <c r="D22" s="3" t="n">
+        <v>2070</v>
+      </c>
+      <c r="E22" s="3" t="inlineStr">
+        <is>
+          <t>R$ 0,17231884057971014</t>
+        </is>
+      </c>
+      <c r="F22" s="3" t="n">
+        <v>1.042296072507553</v>
+      </c>
+      <c r="G22" s="3" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="3" t="inlineStr"/>
+    </row>
+    <row r="24" ht="25" customHeight="1">
+      <c r="A24" s="1" t="inlineStr">
+        <is>
+          <t>[RCK] Campanha de Mensagem</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="2" t="inlineStr">
+        <is>
+          <t>Mes</t>
+        </is>
+      </c>
+      <c r="B25" s="2" t="inlineStr">
+        <is>
+          <t>Investimento</t>
+        </is>
+      </c>
+      <c r="C25" s="2" t="inlineStr">
+        <is>
+          <t>Impressoes</t>
+        </is>
+      </c>
+      <c r="D25" s="2" t="inlineStr">
+        <is>
+          <t>Cliques</t>
+        </is>
+      </c>
+      <c r="E25" s="2" t="inlineStr">
+        <is>
+          <t>CTR</t>
+        </is>
+      </c>
+      <c r="F25" s="2" t="inlineStr">
+        <is>
+          <t>CPC medio</t>
+        </is>
+      </c>
+      <c r="G25" s="2" t="inlineStr">
+        <is>
+          <t>Leads</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="3" t="inlineStr">
+        <is>
+          <t>Setembro</t>
+        </is>
+      </c>
+      <c r="B26" s="3" t="inlineStr">
+        <is>
+          <t>R$ 452,48</t>
+        </is>
+      </c>
+      <c r="C26" s="3" t="n">
+        <v>995</v>
+      </c>
+      <c r="D26" s="3" t="n">
+        <v>1003</v>
+      </c>
+      <c r="E26" s="3" t="inlineStr">
+        <is>
+          <t>R$ 0,45112662013958127</t>
+        </is>
+      </c>
+      <c r="F26" s="3" t="n">
+        <v>1.008040201005025</v>
+      </c>
+      <c r="G26" s="3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="3" t="inlineStr">
+        <is>
+          <t>Agosto</t>
+        </is>
+      </c>
+      <c r="B27" s="3" t="inlineStr">
+        <is>
+          <t>R$ 454,06</t>
+        </is>
+      </c>
+      <c r="C27" s="3" t="n">
+        <v>3309</v>
+      </c>
+      <c r="D27" s="3" t="n">
+        <v>3169</v>
+      </c>
+      <c r="E27" s="3" t="inlineStr">
+        <is>
+          <t>R$ 0,14328179236352162</t>
+        </is>
+      </c>
+      <c r="F27" s="3" t="n">
+        <v>0.9576911453611363</v>
+      </c>
+      <c r="G27" s="3" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="3" t="inlineStr"/>
+    </row>
+    <row r="29">
+      <c r="A29" s="3" t="inlineStr">
+        <is>
+          <t>Agosto</t>
+        </is>
+      </c>
+      <c r="B29" s="3" t="inlineStr">
+        <is>
+          <t>R$ 453,91</t>
+        </is>
+      </c>
+      <c r="C29" s="3" t="n">
+        <v>2119</v>
+      </c>
+      <c r="D29" s="3" t="n">
+        <v>1962</v>
+      </c>
+      <c r="E29" s="3" t="inlineStr">
+        <is>
+          <t>R$ 0,2313506625891947</t>
+        </is>
+      </c>
+      <c r="F29" s="3" t="n">
+        <v>0.92590844738084</v>
+      </c>
+      <c r="G29" s="3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="3" t="inlineStr"/>
+    </row>
+    <row r="31">
+      <c r="A31" s="3" t="inlineStr">
+        <is>
+          <t>Agosto</t>
+        </is>
+      </c>
+      <c r="B31" s="3" t="inlineStr">
+        <is>
+          <t>R$ 452,48</t>
+        </is>
+      </c>
+      <c r="C31" s="3" t="n">
+        <v>995</v>
+      </c>
+      <c r="D31" s="3" t="n">
+        <v>1003</v>
+      </c>
+      <c r="E31" s="3" t="inlineStr">
+        <is>
+          <t>R$ 0,45112662013958127</t>
+        </is>
+      </c>
+      <c r="F31" s="3" t="n">
+        <v>1.008040201005025</v>
+      </c>
+      <c r="G31" s="3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="3" t="inlineStr"/>
+    </row>
+    <row r="33">
+      <c r="A33" s="3" t="inlineStr">
+        <is>
+          <t>Agosto</t>
+        </is>
+      </c>
+      <c r="B33" s="3" t="inlineStr">
+        <is>
+          <t>R$ 356,70</t>
+        </is>
+      </c>
+      <c r="C33" s="3" t="n">
+        <v>1986</v>
+      </c>
+      <c r="D33" s="3" t="n">
+        <v>2070</v>
+      </c>
+      <c r="E33" s="3" t="inlineStr">
+        <is>
+          <t>R$ 0,17231884057971014</t>
+        </is>
+      </c>
+      <c r="F33" s="3" t="n">
+        <v>1.042296072507553</v>
+      </c>
+      <c r="G33" s="3" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="3" t="inlineStr"/>
+    </row>
+    <row r="35" ht="25" customHeight="1">
+      <c r="A35" s="1" t="inlineStr">
+        <is>
+          <t>[RCK] Campanha de Mensagem</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="2" t="inlineStr">
+        <is>
+          <t>Mes</t>
+        </is>
+      </c>
+      <c r="B36" s="2" t="inlineStr">
+        <is>
+          <t>Investimento</t>
+        </is>
+      </c>
+      <c r="C36" s="2" t="inlineStr">
+        <is>
+          <t>Impressoes</t>
+        </is>
+      </c>
+      <c r="D36" s="2" t="inlineStr">
+        <is>
+          <t>Cliques</t>
+        </is>
+      </c>
+      <c r="E36" s="2" t="inlineStr">
+        <is>
+          <t>CTR</t>
+        </is>
+      </c>
+      <c r="F36" s="2" t="inlineStr">
+        <is>
+          <t>CPC medio</t>
+        </is>
+      </c>
+      <c r="G36" s="2" t="inlineStr">
+        <is>
+          <t>Leads</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="3" t="inlineStr">
+        <is>
+          <t>Setembro</t>
+        </is>
+      </c>
+      <c r="B37" s="3" t="inlineStr">
+        <is>
+          <t>R$ 356,70</t>
+        </is>
+      </c>
+      <c r="C37" s="3" t="n">
+        <v>1986</v>
+      </c>
+      <c r="D37" s="3" t="n">
+        <v>2070</v>
+      </c>
+      <c r="E37" s="3" t="inlineStr">
+        <is>
+          <t>R$ 0,17231884057971014</t>
+        </is>
+      </c>
+      <c r="F37" s="3" t="n">
+        <v>1.042296072507553</v>
+      </c>
+      <c r="G37" s="3" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="3" t="inlineStr">
+        <is>
+          <t>Agosto</t>
+        </is>
+      </c>
+      <c r="B38" s="3" t="inlineStr">
+        <is>
+          <t>R$ 454,06</t>
+        </is>
+      </c>
+      <c r="C38" s="3" t="n">
+        <v>3309</v>
+      </c>
+      <c r="D38" s="3" t="n">
+        <v>3169</v>
+      </c>
+      <c r="E38" s="3" t="inlineStr">
+        <is>
+          <t>R$ 0,14328179236352162</t>
+        </is>
+      </c>
+      <c r="F38" s="3" t="n">
+        <v>0.9576911453611363</v>
+      </c>
+      <c r="G38" s="3" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="3" t="inlineStr"/>
+    </row>
+    <row r="40">
+      <c r="A40" s="3" t="inlineStr">
+        <is>
+          <t>Agosto</t>
+        </is>
+      </c>
+      <c r="B40" s="3" t="inlineStr">
+        <is>
+          <t>R$ 453,91</t>
+        </is>
+      </c>
+      <c r="C40" s="3" t="n">
+        <v>2119</v>
+      </c>
+      <c r="D40" s="3" t="n">
+        <v>1962</v>
+      </c>
+      <c r="E40" s="3" t="inlineStr">
+        <is>
+          <t>R$ 0,2313506625891947</t>
+        </is>
+      </c>
+      <c r="F40" s="3" t="n">
+        <v>0.92590844738084</v>
+      </c>
+      <c r="G40" s="3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="3" t="inlineStr"/>
+    </row>
+    <row r="42">
+      <c r="A42" s="3" t="inlineStr">
+        <is>
+          <t>Agosto</t>
+        </is>
+      </c>
+      <c r="B42" s="3" t="inlineStr">
+        <is>
+          <t>R$ 452,48</t>
+        </is>
+      </c>
+      <c r="C42" s="3" t="n">
+        <v>995</v>
+      </c>
+      <c r="D42" s="3" t="n">
+        <v>1003</v>
+      </c>
+      <c r="E42" s="3" t="inlineStr">
+        <is>
+          <t>R$ 0,45112662013958127</t>
+        </is>
+      </c>
+      <c r="F42" s="3" t="n">
+        <v>1.008040201005025</v>
+      </c>
+      <c r="G42" s="3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="3" t="inlineStr"/>
+    </row>
+    <row r="44">
+      <c r="A44" s="3" t="inlineStr">
+        <is>
+          <t>Agosto</t>
+        </is>
+      </c>
+      <c r="B44" s="3" t="inlineStr">
+        <is>
+          <t>R$ 356,70</t>
+        </is>
+      </c>
+      <c r="C44" s="3" t="n">
+        <v>1986</v>
+      </c>
+      <c r="D44" s="3" t="n">
+        <v>2070</v>
+      </c>
+      <c r="E44" s="3" t="inlineStr">
+        <is>
+          <t>R$ 0,17231884057971014</t>
+        </is>
+      </c>
+      <c r="F44" s="3" t="n">
+        <v>1.042296072507553</v>
+      </c>
+      <c r="G44" s="3" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="3" t="inlineStr"/>
+    </row>
+    <row r="46" ht="25" customHeight="1">
+      <c r="A46" s="1" t="inlineStr">
+        <is>
+          <t>[RCK] Geração de Leads 2</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="2" t="inlineStr">
+        <is>
+          <t>Mes</t>
+        </is>
+      </c>
+      <c r="B47" s="2" t="inlineStr">
+        <is>
+          <t>Investimento</t>
+        </is>
+      </c>
+      <c r="C47" s="2" t="inlineStr">
+        <is>
+          <t>Impressoes</t>
+        </is>
+      </c>
+      <c r="D47" s="2" t="inlineStr">
+        <is>
+          <t>Cliques</t>
+        </is>
+      </c>
+      <c r="E47" s="2" t="inlineStr">
+        <is>
+          <t>CTR</t>
+        </is>
+      </c>
+      <c r="F47" s="2" t="inlineStr">
+        <is>
+          <t>CPC medio</t>
+        </is>
+      </c>
+      <c r="G47" s="2" t="inlineStr">
+        <is>
+          <t>Leads</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="3" t="inlineStr">
+        <is>
+          <t>Setembro</t>
+        </is>
+      </c>
+      <c r="B48" s="3" t="inlineStr">
+        <is>
+          <t>R$ 200,00</t>
+        </is>
+      </c>
+      <c r="C48" s="3" t="n">
+        <v>58369</v>
+      </c>
+      <c r="D48" s="3" t="n">
+        <v>58</v>
+      </c>
+      <c r="E48" s="3" t="inlineStr">
+        <is>
+          <t>R$ 3,4482758620689653</t>
+        </is>
+      </c>
+      <c r="F48" s="3" t="n">
+        <v>0.0009936781510733437</v>
+      </c>
+      <c r="G48" s="3" t="n">
+        <v/>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="3" t="inlineStr">
+        <is>
+          <t>Agosto</t>
+        </is>
+      </c>
+      <c r="B49" s="3" t="inlineStr">
+        <is>
+          <t>R$ 200,00</t>
+        </is>
+      </c>
+      <c r="C49" s="3" t="n">
+        <v>58369</v>
+      </c>
+      <c r="D49" s="3" t="n">
+        <v>58</v>
+      </c>
+      <c r="E49" s="3" t="inlineStr">
+        <is>
+          <t>R$ 3,4482758620689653</t>
+        </is>
+      </c>
+      <c r="F49" s="3" t="n">
+        <v>0.0009936781510733437</v>
+      </c>
+      <c r="G49" s="3" t="n">
+        <v/>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="3" t="inlineStr"/>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="A13:G13"/>
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="A35:G35"/>
+    <mergeCell ref="A24:G24"/>
+    <mergeCell ref="A2:G2"/>
+    <mergeCell ref="A46:G46"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>